<commit_message>
EPBDS-2141 add the possibility to use other number types in openl ranges
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/helpers/DoubleRangeRulesParsingTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/helpers/DoubleRangeRulesParsingTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="50">
   <si>
     <t>C1</t>
   </si>
@@ -82,6 +82,94 @@
   </si>
   <si>
     <t>String value</t>
+  </si>
+  <si>
+    <t>getRR(booVal) == val</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>200 .. 300</t>
+  </si>
+  <si>
+    <t>[-100 .. -20)</t>
+  </si>
+  <si>
+    <t>rule4</t>
+  </si>
+  <si>
+    <t>rule5</t>
+  </si>
+  <si>
+    <t>return new BigDecimal(income + 1);</t>
+  </si>
+  <si>
+    <t>Method BigDecimal getBigDecimalValue(double income)</t>
+  </si>
+  <si>
+    <t>getBigDecimalValue(income).longValue()</t>
+  </si>
+  <si>
+    <t>Rules String testLongRange(boolean booVal, double income)</t>
+  </si>
+  <si>
+    <t>Method String getRR(boolean income)</t>
+  </si>
+  <si>
+    <t>if(income) {
+return "Hello";
+} else {
+return "Hello1";
+}</t>
+  </si>
+  <si>
+    <t>Rules String testIntegerRange(boolean booVal, double income)</t>
+  </si>
+  <si>
+    <t>getBigDecimalValue(income).intValue()</t>
+  </si>
+  <si>
+    <t>100 .. 110</t>
+  </si>
+  <si>
+    <t>Rules String testIntegerRange1(boolean booVal, double income)</t>
+  </si>
+  <si>
+    <t>Rules String testByteRange(boolean booVal, double income)</t>
+  </si>
+  <si>
+    <t>20 .. 30</t>
+  </si>
+  <si>
+    <t>50 .. 110</t>
+  </si>
+  <si>
+    <t>Rules String testShortRange(boolean booVal, double income)</t>
+  </si>
+  <si>
+    <t>Rules String testFloatRange(boolean booVal, double income)</t>
+  </si>
+  <si>
+    <t>getBigDecimalValue(income).floatValue()</t>
+  </si>
+  <si>
+    <t>20.5 .. 30.5</t>
+  </si>
+  <si>
+    <t>50.456 .. 110.777</t>
+  </si>
+  <si>
+    <t>400 .. 1110</t>
+  </si>
+  <si>
+    <t>getBigDecimalValue(income).byteValueExact()</t>
+  </si>
+  <si>
+    <t>getBigDecimalValue(income).shortValueExact()</t>
   </si>
 </sst>
 </file>
@@ -145,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +246,14 @@
         <bgColor indexed="22"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -182,6 +276,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -193,7 +300,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +322,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="AFE" xfId="2"/>
@@ -514,27 +642,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:E11"/>
+  <dimension ref="C4:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
     <col min="5" max="5" width="46.85546875" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5">
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="3:9">
+      <c r="C4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="3:5">
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="3:9">
       <c r="C5" s="5" t="s">
         <v>0</v>
       </c>
@@ -544,8 +673,11 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="3:5">
+      <c r="I5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9">
       <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
@@ -555,8 +687,11 @@
       <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:5">
+      <c r="I6" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -567,7 +702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:9">
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
@@ -578,7 +713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:9">
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
@@ -588,8 +723,11 @@
       <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="3:5">
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="61.5" customHeight="1">
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
@@ -599,8 +737,11 @@
       <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="3:5">
+      <c r="I10" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9">
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
@@ -611,9 +752,546 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="3:9">
+      <c r="C14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="3:9">
+      <c r="C15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9">
+      <c r="C16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3">
+        <v>100</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="C22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
+      <c r="C23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="C26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="3:5">
+      <c r="C27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
+      <c r="C28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
+      <c r="C29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
+      <c r="C30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5">
+      <c r="C31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5">
+      <c r="C32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11">
+      <c r="C33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11">
+      <c r="C34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11">
+      <c r="C35" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11">
+      <c r="D38" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="3:11">
+      <c r="D39" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11">
+      <c r="D40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11">
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11">
+      <c r="D42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11">
+      <c r="D43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11">
+      <c r="D44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="16"/>
+    </row>
+    <row r="45" spans="3:11">
+      <c r="D45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11">
+      <c r="D46" s="9"/>
+      <c r="E46" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11">
+      <c r="D47" s="5"/>
+      <c r="E47" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5">
+      <c r="C50" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+    </row>
+    <row r="51" spans="3:5">
+      <c r="C51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5">
+      <c r="C52" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5">
+      <c r="C53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5">
+      <c r="C54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5">
+      <c r="C55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5">
+      <c r="C56" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5">
+      <c r="C57" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5">
+      <c r="C60" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+    </row>
+    <row r="61" spans="3:5">
+      <c r="C61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5">
+      <c r="C62" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5">
+      <c r="C63" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5">
+      <c r="C64" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5">
+      <c r="C65" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5">
+      <c r="C66" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5">
+      <c r="C67" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5">
+      <c r="C70" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="3:5">
+      <c r="C71" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5">
+      <c r="C72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5">
+      <c r="C73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5">
+      <c r="C74" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5">
+      <c r="C75" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5">
+      <c r="C76" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5">
+      <c r="C77" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C70:E70"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="C50:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>